<commit_message>
Add to requirements.txt pandas==1.4.3 protobuf==3.19.1 openpyxl==3.0.10
</commit_message>
<xml_diff>
--- a/lesson14/5ka.xlsx
+++ b/lesson14/5ka.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="229">
   <si>
     <t>count</t>
   </si>
@@ -100,6 +100,9 @@
     <t>Лапша</t>
   </si>
   <si>
+    <t>Коньяк</t>
+  </si>
+  <si>
     <t>Мыло жидкое Чистая линия, для всей семьи, 520 мл</t>
   </si>
   <si>
@@ -157,21 +160,12 @@
     <t>Шоколад Truffles, трюфельный, трюфельный, с начинкой, Коммунарка, 200 г</t>
   </si>
   <si>
-    <t>Шоколад Alpen Gold Max Fun, с кусочками фруктов, 150 г</t>
-  </si>
-  <si>
-    <t>Шоколад Alpen Gold, мармелад-печенье, 150 г</t>
-  </si>
-  <si>
-    <t>Шоколад Alpen Gold Десерт, яблоко-имбирь, 150 г</t>
+    <t>Шоколад Алёнка, молочный, с драже, Красный Октябрь, 90 г</t>
   </si>
   <si>
     <t>Шоколад молочный Merci, 100 г</t>
   </si>
   <si>
-    <t>Шоколад Алёнка, молочный, с драже, Красный Октябрь, 90 г</t>
-  </si>
-  <si>
     <t>Шоколад Alpen Gold, белый, миндаль-кокос, 85 г</t>
   </si>
   <si>
@@ -286,9 +280,6 @@
     <t>Маслины Global Village Selection Hojiblanca*, с косточкой, 160 г *Ходжибланка Глобал Вилледж Селекшн</t>
   </si>
   <si>
-    <t>Маслины Global Village Selection Halkidiki, без косточки, 340 г</t>
-  </si>
-  <si>
     <t>Маслины Global Village Selection Hojiblanca*, без косточки, 160 г *Ходжибланка Глобал Вилледж Селекшн</t>
   </si>
   <si>
@@ -304,9 +295,6 @@
     <t>Антиперспирант Axe, Африка,50 мл</t>
   </si>
   <si>
-    <t>Батончик Nuts, 66 г</t>
-  </si>
-  <si>
     <t>Батончик Gerber*, Doremi, злаковый, фруктовый с яблоком и бананом, с 1 года, 25 г</t>
   </si>
   <si>
@@ -367,9 +355,6 @@
     <t>Пастила Шарлиз, клюква, 220 г</t>
   </si>
   <si>
-    <t>Пастила Белевская, черная смородина, 200 г</t>
-  </si>
-  <si>
     <t>Пастила Шарлиз Белевская, без добавления сахара, 100 г</t>
   </si>
   <si>
@@ -382,6 +367,36 @@
     <t>Лапша Биг Ланч, курица, 90 г</t>
   </si>
   <si>
+    <t>Коньяк Саят Нова, пять звезд, 5 летний, 0,5 л</t>
+  </si>
+  <si>
+    <t>Коньяк Старейшина, российский, пятилетний, 40%, 0,5 л</t>
+  </si>
+  <si>
+    <t>Коньяк Киновский, российский, трёхлетний, 40%, 0,5 л</t>
+  </si>
+  <si>
+    <t>Коньяк Пять Звездочек, российский, пятилетний, 40%, 0,5 л</t>
+  </si>
+  <si>
+    <t>Коньяк Shustoff, российский, пятилетний, 40%, 0,5 л</t>
+  </si>
+  <si>
+    <t>Коньяк Авшар, армянский, пятилетний, 40%, 0,5 л</t>
+  </si>
+  <si>
+    <t>Коньяк Древний Эривань, армянский, десятилетний, 40%, 0,5 л</t>
+  </si>
+  <si>
+    <t>Коньяк Бурсамдзели, 5 летний, 40%, 0,5 л</t>
+  </si>
+  <si>
+    <t>Коньяк Galavani, грузинский, восьмилетний, 40%, 0,5 л</t>
+  </si>
+  <si>
+    <t>Коньяк Couiturier Vsop, 5 летний, 0,5 л</t>
+  </si>
+  <si>
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/dhv76qmrwrmxz4bcbil2yuwgb4.jpg</t>
   </si>
   <si>
@@ -439,21 +454,12 @@
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/kdmtgtksawn6lji543tiokeysu.jpg</t>
   </si>
   <si>
-    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/kpan24xvt2et75igshrnd574ee.jpg</t>
-  </si>
-  <si>
-    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/vlqkn7eovlllib2zoqb73p64fe.jpg</t>
-  </si>
-  <si>
-    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/3sn2selttyjnv3m5ebw5txuklu.jpg</t>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/6p3ctm2iailk3xerkkwj2oqixe.jpg</t>
   </si>
   <si>
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/tsmtczvjbjr6fkw4ghu6ktu23i.jpg</t>
   </si>
   <si>
-    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/6p3ctm2iailk3xerkkwj2oqixe.jpg</t>
-  </si>
-  <si>
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/fvqql2hgovceyykiloh2ilmf6m.jpg</t>
   </si>
   <si>
@@ -568,9 +574,6 @@
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/fpet6234umko5qim7znicyu6li.jpg</t>
   </si>
   <si>
-    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/2bkqubvc2ba763cqktsjsfsf2m.jpg</t>
-  </si>
-  <si>
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/53d3vxlkzt7ik7klwoejdkn2bm.jpg</t>
   </si>
   <si>
@@ -580,15 +583,12 @@
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/ipoiodojcwsthigkzssudqk2uu.jpg</t>
   </si>
   <si>
-    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/c53dtlq4nvmgpe57iwfyythcgy.jpg</t>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/z4j2ssxbmffd67i7z4acxl53vi.jpg</t>
   </si>
   <si>
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/7wiyr7reepigr67q6f567cigry.jpg</t>
   </si>
   <si>
-    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/q66vkvftudyxc6uxhp5yqcbdce.jpg</t>
-  </si>
-  <si>
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/fxxdtds5apntvzuziecrcc5crq.jpg</t>
   </si>
   <si>
@@ -649,9 +649,6 @@
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/y5eruhhnti6o3txyppnd6idffu.jpg</t>
   </si>
   <si>
-    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/oejv5nen53pwfnhbz3cmva3u7a.jpg</t>
-  </si>
-  <si>
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/vlvey6s5dqyqmqcprvqilhmfe4.jpg</t>
   </si>
   <si>
@@ -662,6 +659,36 @@
   </si>
   <si>
     <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/jeqgmn7o37osvvzz5ttypgc4oe.jpg</t>
+  </si>
+  <si>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/3bxpycsfi4nhzwicmby2i4h2ni.jpg</t>
+  </si>
+  <si>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/wd4ofqx2cneborwx3shojoyd2y.jpg</t>
+  </si>
+  <si>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/qhnuxlhtb5y3disdzlpdrfx5s4.jpg</t>
+  </si>
+  <si>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/34dvzbuygosyqkqwk2hjv67hku.jpg</t>
+  </si>
+  <si>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/trueajj6d6zp6jbjrxevi3si6a.jpg</t>
+  </si>
+  <si>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/235z7zqzmj455xpnsismjissym.jpg</t>
+  </si>
+  <si>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/eixom2b65varg5kkw776nweuim.jpg</t>
+  </si>
+  <si>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/wxp5q32rpvqv4uu6qhi35ukea4.jpg</t>
+  </si>
+  <si>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/eps7z5roofjphhr7pnycewm7wu.jpg</t>
+  </si>
+  <si>
+    <t>https://leonardo.edadeal.io/dyn/cr/catalyst/offers/iiihputxzj4mbdxtya6e36fzry.jpg</t>
   </si>
   <si>
     <t>2022-08-01T00:00:00Z</t>
@@ -1044,7 +1071,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J95"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1084,16 +1111,16 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E2">
         <v>269.99</v>
@@ -1108,24 +1135,24 @@
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J2" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E3">
         <v>267.99</v>
@@ -1140,24 +1167,24 @@
         <v>41</v>
       </c>
       <c r="I3" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J3" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E4">
         <v>267.99</v>
@@ -1172,24 +1199,24 @@
         <v>41</v>
       </c>
       <c r="I4" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J4" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E5">
         <v>254.99</v>
@@ -1204,24 +1231,24 @@
         <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J5" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="E6">
         <v>254.99</v>
@@ -1236,24 +1263,24 @@
         <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J6" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E7">
         <v>129.99</v>
@@ -1268,24 +1295,24 @@
         <v>47</v>
       </c>
       <c r="I7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J7" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E8">
         <v>129.99</v>
@@ -1300,24 +1327,24 @@
         <v>47</v>
       </c>
       <c r="I8" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J8" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="E9">
         <v>129.99</v>
@@ -1332,10 +1359,10 @@
         <v>47</v>
       </c>
       <c r="I9" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J9" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1346,10 +1373,10 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E10">
         <v>259.99</v>
@@ -1364,24 +1391,24 @@
         <v>43</v>
       </c>
       <c r="I10" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J10" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E11">
         <v>109.99</v>
@@ -1396,24 +1423,24 @@
         <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J11" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E12">
         <v>93.98999999999999</v>
@@ -1428,24 +1455,24 @@
         <v>37</v>
       </c>
       <c r="I12" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J12" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E13">
         <v>215.99</v>
@@ -1460,24 +1487,24 @@
         <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J13" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E14">
         <v>93.98999999999999</v>
@@ -1492,10 +1519,10 @@
         <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J14" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1506,10 +1533,10 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E15">
         <v>129.99</v>
@@ -1524,24 +1551,24 @@
         <v>39</v>
       </c>
       <c r="I15" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J15" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="E16">
         <v>99.98999999999999</v>
@@ -1556,10 +1583,10 @@
         <v>31</v>
       </c>
       <c r="I16" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J16" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1570,10 +1597,10 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E17">
         <v>129.99</v>
@@ -1588,24 +1615,24 @@
         <v>39</v>
       </c>
       <c r="I17" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J17" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="F18">
         <v>99.98999999999999</v>
@@ -1614,10 +1641,10 @@
         <v>150</v>
       </c>
       <c r="I18" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J18" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1628,10 +1655,10 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E19">
         <v>179.99</v>
@@ -1646,24 +1673,24 @@
         <v>28</v>
       </c>
       <c r="I19" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J19" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E20">
         <v>215.99</v>
@@ -1678,172 +1705,184 @@
         <v>31</v>
       </c>
       <c r="I20" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J20" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
+      </c>
+      <c r="E21">
+        <v>129.99</v>
       </c>
       <c r="F21">
-        <v>99.98999999999999</v>
+        <v>79.98999999999999</v>
       </c>
       <c r="G21">
-        <v>150</v>
+        <v>90</v>
+      </c>
+      <c r="H21">
+        <v>39</v>
       </c>
       <c r="I21" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J21" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22">
-        <v>500</v>
+        <v>531</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>142</v>
+        <v>147</v>
+      </c>
+      <c r="E22">
+        <v>199.99</v>
       </c>
       <c r="F22">
-        <v>99.98999999999999</v>
+        <v>149.99</v>
       </c>
       <c r="G22">
-        <v>150</v>
+        <v>100</v>
+      </c>
+      <c r="H22">
+        <v>26</v>
       </c>
       <c r="I22" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J22" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>508</v>
+        <v>565</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E23">
-        <v>179.99</v>
+        <v>93.98999999999999</v>
       </c>
       <c r="F23">
-        <v>129.99</v>
+        <v>59.99</v>
       </c>
       <c r="G23">
-        <v>150</v>
+        <v>85</v>
       </c>
       <c r="H23">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="I23" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J23" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>535</v>
+        <v>614</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E24">
-        <v>199.99</v>
+        <v>154.99</v>
       </c>
       <c r="F24">
-        <v>149.99</v>
+        <v>109.99</v>
       </c>
       <c r="G24">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H24">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I24" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J24" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>555</v>
+        <v>655</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E25">
-        <v>129.99</v>
+        <v>109.99</v>
       </c>
       <c r="F25">
-        <v>79.98999999999999</v>
+        <v>69.98999999999999</v>
       </c>
       <c r="G25">
         <v>90</v>
       </c>
       <c r="H25">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I25" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J25" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>569</v>
+        <v>667</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E26">
         <v>93.98999999999999</v>
@@ -1858,88 +1897,88 @@
         <v>37</v>
       </c>
       <c r="I26" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J26" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
-        <v>617</v>
+        <v>697</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E27">
-        <v>154.99</v>
+        <v>93.98999999999999</v>
       </c>
       <c r="F27">
-        <v>109.99</v>
+        <v>59.99</v>
       </c>
       <c r="G27">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H27">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I27" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J27" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28">
-        <v>657</v>
+        <v>698</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="E28">
-        <v>109.99</v>
+        <v>179.99</v>
       </c>
       <c r="F28">
-        <v>69.98999999999999</v>
+        <v>129.99</v>
       </c>
       <c r="G28">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="H28">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="I28" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J28" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29">
-        <v>667</v>
+        <v>704</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E29">
         <v>93.98999999999999</v>
@@ -1954,24 +1993,24 @@
         <v>37</v>
       </c>
       <c r="I29" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J29" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30">
-        <v>699</v>
+        <v>748</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E30">
         <v>93.98999999999999</v>
@@ -1986,88 +2025,88 @@
         <v>37</v>
       </c>
       <c r="I30" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J30" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31">
-        <v>700</v>
+        <v>756</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E31">
-        <v>179.99</v>
+        <v>215.99</v>
       </c>
       <c r="F31">
-        <v>129.99</v>
+        <v>149.99</v>
       </c>
       <c r="G31">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H31">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I31" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J31" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32">
-        <v>709</v>
+        <v>837</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E32">
-        <v>93.98999999999999</v>
+        <v>109.99</v>
       </c>
       <c r="F32">
-        <v>59.99</v>
+        <v>69.98999999999999</v>
       </c>
       <c r="G32">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H32">
         <v>37</v>
       </c>
       <c r="I32" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J32" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33">
-        <v>751</v>
+        <v>964</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E33">
         <v>93.98999999999999</v>
@@ -2076,382 +2115,382 @@
         <v>59.99</v>
       </c>
       <c r="G33">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H33">
         <v>37</v>
       </c>
       <c r="I33" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J33" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34">
-        <v>759</v>
+        <v>981</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E34">
-        <v>215.99</v>
+        <v>141.99</v>
       </c>
       <c r="F34">
-        <v>149.99</v>
+        <v>89.98999999999999</v>
       </c>
       <c r="G34">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H34">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="I34" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J34" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35">
-        <v>840</v>
+        <v>997</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E35">
-        <v>109.99</v>
+        <v>79.98999999999999</v>
       </c>
       <c r="F35">
         <v>69.98999999999999</v>
       </c>
       <c r="G35">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H35">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="I35" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J35" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36">
-        <v>965</v>
+        <v>463</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="E36">
-        <v>93.98999999999999</v>
+        <v>169.99</v>
       </c>
       <c r="F36">
-        <v>59.99</v>
+        <v>134.99</v>
       </c>
       <c r="G36">
-        <v>80</v>
+        <v>350</v>
       </c>
       <c r="H36">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="I36" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J36" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37">
-        <v>981</v>
+        <v>419</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="E37">
-        <v>141.99</v>
+        <v>325.99</v>
       </c>
       <c r="F37">
-        <v>89.98999999999999</v>
+        <v>219.99</v>
       </c>
       <c r="G37">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="H37">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I37" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J37" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38">
-        <v>996</v>
+        <v>970</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E38">
-        <v>79.98999999999999</v>
+        <v>267.99</v>
       </c>
       <c r="F38">
-        <v>69.98999999999999</v>
+        <v>209.99</v>
       </c>
       <c r="G38">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="H38">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I38" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J38" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39">
-        <v>463</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E39">
-        <v>169.99</v>
+        <v>379.99</v>
       </c>
       <c r="F39">
-        <v>134.99</v>
+        <v>249.99</v>
       </c>
       <c r="G39">
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="H39">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="I39" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J39" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40">
-        <v>418</v>
+        <v>319</v>
       </c>
       <c r="B40" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E40">
-        <v>325.99</v>
+        <v>249.99</v>
       </c>
       <c r="F40">
-        <v>219.99</v>
+        <v>179.99</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="H40">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I40" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J40" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41">
-        <v>967</v>
+        <v>696</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E41">
-        <v>267.99</v>
+        <v>249.99</v>
       </c>
       <c r="F41">
-        <v>209.99</v>
+        <v>179.99</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="H41">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I41" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J41" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42">
-        <v>66</v>
+        <v>237</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="E42">
-        <v>379.99</v>
+        <v>89.98999999999999</v>
       </c>
       <c r="F42">
-        <v>249.99</v>
+        <v>79.98999999999999</v>
       </c>
       <c r="G42">
-        <v>150</v>
+        <v>450</v>
       </c>
       <c r="H42">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="I42" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J42" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43">
-        <v>320</v>
+        <v>581</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E43">
-        <v>249.99</v>
+        <v>89.98999999999999</v>
       </c>
       <c r="F43">
-        <v>179.99</v>
+        <v>79.98999999999999</v>
       </c>
       <c r="G43">
-        <v>150</v>
+        <v>450</v>
       </c>
       <c r="H43">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="I43" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J43" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44">
-        <v>698</v>
+        <v>623</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E44">
-        <v>249.99</v>
+        <v>89.98999999999999</v>
       </c>
       <c r="F44">
-        <v>179.99</v>
+        <v>79.98999999999999</v>
       </c>
       <c r="G44">
-        <v>150</v>
+        <v>450</v>
       </c>
       <c r="H44">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="I44" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J44" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45">
-        <v>239</v>
+        <v>692</v>
       </c>
       <c r="B45" t="s">
         <v>16</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="E45">
         <v>89.98999999999999</v>
@@ -2466,24 +2505,24 @@
         <v>12</v>
       </c>
       <c r="I45" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J45" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46">
-        <v>583</v>
+        <v>782</v>
       </c>
       <c r="B46" t="s">
         <v>16</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E46">
         <v>89.98999999999999</v>
@@ -2498,1575 +2537,1703 @@
         <v>12</v>
       </c>
       <c r="I46" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J46" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47">
-        <v>625</v>
+        <v>428</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E47">
-        <v>89.98999999999999</v>
+        <v>159.99</v>
       </c>
       <c r="F47">
-        <v>79.98999999999999</v>
+        <v>109.99</v>
       </c>
       <c r="G47">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="H47">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="I47" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J47" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48">
-        <v>692</v>
+        <v>615</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E48">
-        <v>89.98999999999999</v>
+        <v>149.99</v>
       </c>
       <c r="F48">
-        <v>79.98999999999999</v>
+        <v>134.99</v>
       </c>
       <c r="G48">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="H48">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I48" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J48" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49">
-        <v>784</v>
+        <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E49">
-        <v>89.98999999999999</v>
+        <v>336.99</v>
       </c>
       <c r="F49">
-        <v>79.98999999999999</v>
+        <v>199.9</v>
       </c>
       <c r="G49">
-        <v>450</v>
+        <v>12</v>
       </c>
       <c r="H49">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="I49" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J49" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50">
-        <v>428</v>
+        <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E50">
-        <v>159.99</v>
+        <v>174.99</v>
       </c>
       <c r="F50">
-        <v>109.99</v>
+        <v>139.99</v>
       </c>
       <c r="G50">
-        <v>250</v>
+        <v>4</v>
       </c>
       <c r="H50">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="I50" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J50" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51">
-        <v>616</v>
+        <v>513</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C51" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="E51">
-        <v>149.99</v>
+        <v>249.99</v>
       </c>
       <c r="F51">
-        <v>134.99</v>
+        <v>199.99</v>
       </c>
       <c r="G51">
-        <v>300</v>
+        <v>4</v>
       </c>
       <c r="H51">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="I51" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J51" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52">
-        <v>0</v>
+        <v>519</v>
       </c>
       <c r="B52" t="s">
         <v>18</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="E52">
-        <v>336.99</v>
+        <v>409.99</v>
       </c>
       <c r="F52">
-        <v>199.9</v>
+        <v>329.99</v>
       </c>
       <c r="G52">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H52">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I52" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J52" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E53">
-        <v>174.99</v>
+        <v>139.99</v>
       </c>
       <c r="F53">
-        <v>139.99</v>
+        <v>109.99</v>
       </c>
       <c r="G53">
-        <v>4</v>
+        <v>300</v>
       </c>
       <c r="H53">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I53" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J53" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54">
-        <v>516</v>
+        <v>357</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E54">
-        <v>249.99</v>
+        <v>219.99</v>
       </c>
       <c r="F54">
-        <v>199.99</v>
+        <v>149.99</v>
       </c>
       <c r="G54">
-        <v>4</v>
+        <v>314</v>
       </c>
       <c r="H54">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="I54" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J54" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55">
-        <v>523</v>
+        <v>808</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="E55">
-        <v>409.99</v>
+        <v>219.99</v>
       </c>
       <c r="F55">
-        <v>329.99</v>
+        <v>149.99</v>
       </c>
       <c r="G55">
-        <v>8</v>
+        <v>314</v>
       </c>
       <c r="H55">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="I55" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J55" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56">
-        <v>217</v>
+        <v>882</v>
       </c>
       <c r="B56" t="s">
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="E56">
-        <v>139.99</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="F56">
-        <v>109.99</v>
+        <v>89.98999999999999</v>
       </c>
       <c r="G56">
         <v>300</v>
       </c>
       <c r="H56">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I56" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J56" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57">
-        <v>359</v>
+        <v>982</v>
       </c>
       <c r="B57" t="s">
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="E57">
-        <v>219.99</v>
+        <v>177.99</v>
       </c>
       <c r="F57">
-        <v>149.99</v>
+        <v>139.99</v>
       </c>
       <c r="G57">
-        <v>314</v>
+        <v>340</v>
       </c>
       <c r="H57">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="I57" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J57" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58">
-        <v>809</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="E58">
-        <v>219.99</v>
+        <v>129.99</v>
       </c>
       <c r="F58">
-        <v>149.99</v>
+        <v>86.98999999999999</v>
       </c>
       <c r="G58">
-        <v>314</v>
+        <v>425</v>
       </c>
       <c r="H58">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I58" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J58" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59">
-        <v>885</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C59" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="E59">
-        <v>99.98999999999999</v>
+        <v>129.99</v>
       </c>
       <c r="F59">
-        <v>89.98999999999999</v>
+        <v>86.98999999999999</v>
       </c>
       <c r="G59">
-        <v>300</v>
+        <v>425</v>
       </c>
       <c r="H59">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="I59" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J59" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60">
-        <v>984</v>
+        <v>142</v>
       </c>
       <c r="B60" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C60" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E60">
-        <v>177.99</v>
+        <v>89.98999999999999</v>
       </c>
       <c r="F60">
-        <v>139.99</v>
+        <v>79.98999999999999</v>
       </c>
       <c r="G60">
-        <v>340</v>
+        <v>160</v>
       </c>
       <c r="H60">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I60" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J60" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61">
-        <v>58</v>
+        <v>886</v>
       </c>
       <c r="B61" t="s">
         <v>20</v>
       </c>
       <c r="C61" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="E61">
-        <v>129.99</v>
+        <v>94.98999999999999</v>
       </c>
       <c r="F61">
-        <v>86.98999999999999</v>
+        <v>84.98999999999999</v>
       </c>
       <c r="G61">
-        <v>425</v>
+        <v>160</v>
       </c>
       <c r="H61">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="I61" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J61" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62">
-        <v>59</v>
+        <v>273</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C62" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="E62">
-        <v>129.99</v>
+        <v>119.99</v>
       </c>
       <c r="F62">
-        <v>86.98999999999999</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="G62">
-        <v>425</v>
+        <v>400</v>
       </c>
       <c r="H62">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="I62" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J62" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63">
-        <v>142</v>
+        <v>457</v>
       </c>
       <c r="B63" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C63" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="E63">
-        <v>89.98999999999999</v>
+        <v>69.98999999999999</v>
       </c>
       <c r="F63">
-        <v>79.98999999999999</v>
+        <v>59.99</v>
       </c>
       <c r="G63">
-        <v>160</v>
+        <v>400</v>
       </c>
       <c r="H63">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I63" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J63" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="B64" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="E64">
-        <v>177.99</v>
+        <v>45.99</v>
       </c>
       <c r="F64">
-        <v>139.99</v>
-      </c>
-      <c r="G64">
-        <v>340</v>
+        <v>39.99</v>
       </c>
       <c r="H64">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="I64" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J64" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65">
-        <v>889</v>
+        <v>26</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="E65">
-        <v>94.98999999999999</v>
+        <v>379.99</v>
       </c>
       <c r="F65">
-        <v>84.98999999999999</v>
+        <v>249.99</v>
       </c>
       <c r="G65">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="H65">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="I65" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J65" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66">
-        <v>276</v>
+        <v>129</v>
       </c>
       <c r="B66" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C66" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E66">
-        <v>119.99</v>
+        <v>96.98999999999999</v>
       </c>
       <c r="F66">
-        <v>99.98999999999999</v>
+        <v>75.98999999999999</v>
       </c>
       <c r="G66">
-        <v>400</v>
+        <v>25</v>
       </c>
       <c r="H66">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I66" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J66" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67">
-        <v>456</v>
+        <v>153</v>
       </c>
       <c r="B67" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C67" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="E67">
-        <v>69.98999999999999</v>
+        <v>919.99</v>
       </c>
       <c r="F67">
-        <v>59.99</v>
+        <v>649.99</v>
       </c>
       <c r="G67">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="H67">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I67" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J67" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68">
-        <v>512</v>
+        <v>191</v>
       </c>
       <c r="B68" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E68">
         <v>59.99</v>
       </c>
       <c r="F68">
-        <v>53.99</v>
+        <v>44.99</v>
+      </c>
+      <c r="G68">
+        <v>52</v>
       </c>
       <c r="H68">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="I68" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J68" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69">
-        <v>45</v>
+        <v>453</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C69" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E69">
-        <v>379.99</v>
+        <v>604.99</v>
       </c>
       <c r="F69">
-        <v>249.99</v>
+        <v>399.99</v>
       </c>
       <c r="G69">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H69">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I69" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J69" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70">
-        <v>83</v>
+        <v>803</v>
       </c>
       <c r="B70" t="s">
         <v>23</v>
       </c>
       <c r="C70" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="E70">
-        <v>88.19</v>
+        <v>29.49</v>
       </c>
       <c r="F70">
-        <v>44.9</v>
+        <v>16.99</v>
       </c>
       <c r="G70">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="H70">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I70" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J70" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71">
-        <v>130</v>
+        <v>369</v>
       </c>
       <c r="B71" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="E71">
-        <v>96.98999999999999</v>
+        <v>50.19</v>
       </c>
       <c r="F71">
-        <v>75.98999999999999</v>
+        <v>24.99</v>
       </c>
       <c r="G71">
         <v>25</v>
       </c>
       <c r="H71">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="I71" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J71" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72">
-        <v>154</v>
+        <v>533</v>
       </c>
       <c r="B72" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E72">
-        <v>919.99</v>
+        <v>50.19</v>
       </c>
       <c r="F72">
-        <v>649.99</v>
+        <v>24.99</v>
       </c>
       <c r="G72">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="H72">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="I72" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J72" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73">
-        <v>194</v>
+        <v>730</v>
       </c>
       <c r="B73" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C73" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="E73">
-        <v>59.99</v>
+        <v>72.48999999999999</v>
       </c>
       <c r="F73">
-        <v>44.99</v>
+        <v>34.99</v>
       </c>
       <c r="G73">
+        <v>25</v>
+      </c>
+      <c r="H73">
         <v>52</v>
       </c>
-      <c r="H73">
-        <v>26</v>
-      </c>
       <c r="I73" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J73" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74">
-        <v>454</v>
+        <v>771</v>
       </c>
       <c r="B74" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C74" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E74">
-        <v>604.99</v>
+        <v>50.19</v>
       </c>
       <c r="F74">
-        <v>399.99</v>
+        <v>24.99</v>
       </c>
       <c r="G74">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="H74">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="I74" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J74" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75">
-        <v>805</v>
+        <v>846</v>
       </c>
       <c r="B75" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C75" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="E75">
-        <v>29.49</v>
+        <v>50.19</v>
       </c>
       <c r="F75">
-        <v>16.99</v>
+        <v>24.99</v>
       </c>
       <c r="G75">
-        <v>40</v>
+        <v>24.5</v>
       </c>
       <c r="H75">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="I75" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J75" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76">
-        <v>370</v>
+        <v>979</v>
       </c>
       <c r="B76" t="s">
         <v>24</v>
       </c>
       <c r="C76" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="E76">
-        <v>50.19</v>
+        <v>21.99</v>
       </c>
       <c r="F76">
-        <v>24.99</v>
+        <v>16.99</v>
       </c>
       <c r="G76">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H76">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="I76" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J76" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77">
-        <v>536</v>
+        <v>91</v>
       </c>
       <c r="B77" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C77" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="E77">
-        <v>50.19</v>
+        <v>329.99</v>
       </c>
       <c r="F77">
-        <v>24.99</v>
+        <v>199.99</v>
       </c>
       <c r="G77">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="H77">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I77" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J77" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78">
-        <v>733</v>
+        <v>248</v>
       </c>
       <c r="B78" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C78" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="E78">
-        <v>72.48999999999999</v>
+        <v>109.99</v>
       </c>
       <c r="F78">
-        <v>34.99</v>
+        <v>95.98999999999999</v>
       </c>
       <c r="G78">
-        <v>25</v>
+        <v>240</v>
       </c>
       <c r="H78">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="I78" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J78" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79">
-        <v>773</v>
+        <v>259</v>
       </c>
       <c r="B79" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C79" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="E79">
-        <v>50.19</v>
+        <v>229.99</v>
       </c>
       <c r="F79">
-        <v>24.99</v>
+        <v>169.99</v>
       </c>
       <c r="G79">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="H79">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="I79" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J79" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80">
-        <v>849</v>
+        <v>353</v>
       </c>
       <c r="B80" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C80" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E80">
-        <v>50.19</v>
+        <v>69.98999999999999</v>
       </c>
       <c r="F80">
-        <v>24.99</v>
+        <v>62.99</v>
       </c>
       <c r="G80">
-        <v>24.5</v>
+        <v>180</v>
       </c>
       <c r="H80">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="I80" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J80" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81">
-        <v>979</v>
+        <v>445</v>
       </c>
       <c r="B81" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E81">
-        <v>21.99</v>
+        <v>69.98999999999999</v>
       </c>
       <c r="F81">
-        <v>16.99</v>
+        <v>62.99</v>
       </c>
       <c r="G81">
-        <v>17</v>
+        <v>180</v>
       </c>
       <c r="H81">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="I81" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="J81" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82">
-        <v>96</v>
+        <v>461</v>
       </c>
       <c r="B82" t="s">
         <v>25</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E82">
-        <v>329.99</v>
+        <v>69.98999999999999</v>
       </c>
       <c r="F82">
-        <v>199.99</v>
+        <v>62.99</v>
       </c>
       <c r="G82">
-        <v>250</v>
+        <v>180</v>
       </c>
       <c r="H82">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="I82" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J82" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83">
-        <v>250</v>
+        <v>739</v>
       </c>
       <c r="B83" t="s">
         <v>25</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="E83">
-        <v>109.99</v>
+        <v>399.99</v>
       </c>
       <c r="F83">
-        <v>95.98999999999999</v>
+        <v>359.99</v>
       </c>
       <c r="G83">
-        <v>240</v>
+        <v>100</v>
       </c>
       <c r="H83">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I83" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J83" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84">
-        <v>260</v>
+        <v>137</v>
       </c>
       <c r="B84" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C84" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="E84">
-        <v>229.99</v>
+        <v>74.98999999999999</v>
       </c>
       <c r="F84">
-        <v>169.99</v>
+        <v>66.98999999999999</v>
       </c>
       <c r="G84">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="H84">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="I84" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J84" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85">
-        <v>354</v>
+        <v>447</v>
       </c>
       <c r="B85" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C85" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E85">
-        <v>69.98999999999999</v>
+        <v>74.98999999999999</v>
       </c>
       <c r="F85">
-        <v>62.99</v>
+        <v>66.98999999999999</v>
       </c>
       <c r="G85">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="H85">
         <v>11</v>
       </c>
       <c r="I85" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J85" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86">
-        <v>445</v>
+        <v>921</v>
       </c>
       <c r="B86" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C86" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E86">
-        <v>69.98999999999999</v>
+        <v>109.99</v>
       </c>
       <c r="F86">
-        <v>62.99</v>
+        <v>98.98999999999999</v>
       </c>
       <c r="G86">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="H86">
         <v>11</v>
       </c>
       <c r="I86" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J86" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87">
-        <v>460</v>
+        <v>338</v>
       </c>
       <c r="B87" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C87" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E87">
-        <v>69.98999999999999</v>
+        <v>109.99</v>
       </c>
       <c r="F87">
-        <v>62.99</v>
+        <v>89.98999999999999</v>
       </c>
       <c r="G87">
-        <v>180</v>
+        <v>500</v>
       </c>
       <c r="H87">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="I87" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="J87" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88">
-        <v>741</v>
+        <v>602</v>
       </c>
       <c r="B88" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C88" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="E88">
-        <v>399.99</v>
+        <v>169.99</v>
       </c>
       <c r="F88">
-        <v>359.99</v>
+        <v>114.99</v>
       </c>
       <c r="G88">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="H88">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="I88" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J88" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89">
-        <v>140</v>
+        <v>789</v>
       </c>
       <c r="B89" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C89" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="E89">
-        <v>74.98999999999999</v>
+        <v>69.98999999999999</v>
       </c>
       <c r="F89">
-        <v>66.98999999999999</v>
+        <v>52.99</v>
       </c>
       <c r="G89">
-        <v>220</v>
+        <v>90</v>
       </c>
       <c r="H89">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I89" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J89" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90">
-        <v>447</v>
+        <v>130</v>
       </c>
       <c r="B90" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C90" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E90">
-        <v>74.98999999999999</v>
+        <v>749.99</v>
       </c>
       <c r="F90">
-        <v>66.98999999999999</v>
+        <v>589.99</v>
       </c>
       <c r="G90">
-        <v>220</v>
+        <v>0.5</v>
       </c>
       <c r="H90">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I90" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J90" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91">
-        <v>497</v>
+        <v>297</v>
       </c>
       <c r="B91" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C91" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E91">
-        <v>249.99</v>
+        <v>769.99</v>
       </c>
       <c r="F91">
-        <v>179.99</v>
+        <v>599.99</v>
       </c>
       <c r="G91">
-        <v>200</v>
+        <v>0.5</v>
       </c>
       <c r="H91">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I91" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J91" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92">
-        <v>932</v>
+        <v>329</v>
       </c>
       <c r="B92" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C92" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E92">
-        <v>109.99</v>
+        <v>629.99</v>
       </c>
       <c r="F92">
-        <v>98.98999999999999</v>
+        <v>529.99</v>
       </c>
       <c r="G92">
-        <v>100</v>
+        <v>0.5</v>
       </c>
       <c r="H92">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I92" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J92" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93">
-        <v>341</v>
+        <v>365</v>
       </c>
       <c r="B93" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C93" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E93">
-        <v>109.99</v>
+        <v>819.99</v>
       </c>
       <c r="F93">
-        <v>89.98999999999999</v>
+        <v>669.99</v>
       </c>
       <c r="G93">
-        <v>500</v>
+        <v>0.5</v>
       </c>
       <c r="H93">
         <v>19</v>
       </c>
       <c r="I93" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="J93" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94">
-        <v>604</v>
+        <v>502</v>
       </c>
       <c r="B94" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C94" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E94">
-        <v>169.99</v>
+        <v>619.99</v>
       </c>
       <c r="F94">
-        <v>114.99</v>
+        <v>499.99</v>
       </c>
       <c r="G94">
-        <v>300</v>
+        <v>0.5</v>
       </c>
       <c r="H94">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I94" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J94" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95">
-        <v>792</v>
+        <v>637</v>
       </c>
       <c r="B95" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C95" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E95">
-        <v>69.98999999999999</v>
+        <v>619.99</v>
       </c>
       <c r="F95">
-        <v>52.99</v>
+        <v>519.99</v>
       </c>
       <c r="G95">
-        <v>90</v>
+        <v>0.5</v>
       </c>
       <c r="H95">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="I95" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="J95" t="s">
-        <v>218</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96">
+        <v>657</v>
+      </c>
+      <c r="B96" t="s">
+        <v>28</v>
+      </c>
+      <c r="C96" t="s">
+        <v>123</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E96">
+        <v>849.99</v>
+      </c>
+      <c r="F96">
+        <v>699.99</v>
+      </c>
+      <c r="G96">
+        <v>0.5</v>
+      </c>
+      <c r="H96">
+        <v>18</v>
+      </c>
+      <c r="I96" t="s">
+        <v>225</v>
+      </c>
+      <c r="J96" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97">
+        <v>701</v>
+      </c>
+      <c r="B97" t="s">
+        <v>28</v>
+      </c>
+      <c r="C97" t="s">
+        <v>124</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E97">
+        <v>649.99</v>
+      </c>
+      <c r="F97">
+        <v>499.99</v>
+      </c>
+      <c r="G97">
+        <v>0.5</v>
+      </c>
+      <c r="H97">
+        <v>24</v>
+      </c>
+      <c r="I97" t="s">
+        <v>225</v>
+      </c>
+      <c r="J97" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98">
+        <v>702</v>
+      </c>
+      <c r="B98" t="s">
+        <v>28</v>
+      </c>
+      <c r="C98" t="s">
+        <v>125</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E98">
+        <v>799.99</v>
+      </c>
+      <c r="F98">
+        <v>649.99</v>
+      </c>
+      <c r="G98">
+        <v>0.5</v>
+      </c>
+      <c r="H98">
+        <v>19</v>
+      </c>
+      <c r="I98" t="s">
+        <v>225</v>
+      </c>
+      <c r="J98" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99">
+        <v>746</v>
+      </c>
+      <c r="B99" t="s">
+        <v>28</v>
+      </c>
+      <c r="C99" t="s">
+        <v>126</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E99">
+        <v>649.99</v>
+      </c>
+      <c r="F99">
+        <v>549.99</v>
+      </c>
+      <c r="G99">
+        <v>0.5</v>
+      </c>
+      <c r="H99">
+        <v>16</v>
+      </c>
+      <c r="I99" t="s">
+        <v>225</v>
+      </c>
+      <c r="J99" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -4165,6 +4332,10 @@
     <hyperlink ref="D93" r:id="rId92"/>
     <hyperlink ref="D94" r:id="rId93"/>
     <hyperlink ref="D95" r:id="rId94"/>
+    <hyperlink ref="D96" r:id="rId95"/>
+    <hyperlink ref="D97" r:id="rId96"/>
+    <hyperlink ref="D98" r:id="rId97"/>
+    <hyperlink ref="D99" r:id="rId98"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>